<commit_message>
moved impaq to west coat random
</commit_message>
<xml_diff>
--- a/2018_2025_Summary.xlsx
+++ b/2018_2025_Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/61c36765f8dc212b/Desktop/ExpoFinal Report/map_site/All_Schools_Map/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{90265CFE-C118-4322-A6D5-4B6675F4C7ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BEE3B30A-0398-4E04-ACEC-CE7EB103E915}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{90265CFE-C118-4322-A6D5-4B6675F4C7ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E5D6EA4-A621-43F2-B3D1-E035605042E0}"/>
   <bookViews>
-    <workbookView xWindow="2573" yWindow="2573" windowWidth="16199" windowHeight="9307" xr2:uid="{F387CA26-9EC5-48FA-B22C-D720BB427D09}"/>
+    <workbookView xWindow="2940" yWindow="2940" windowWidth="16200" windowHeight="9307" xr2:uid="{F387CA26-9EC5-48FA-B22C-D720BB427D09}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="286">
   <si>
     <t>REGION</t>
   </si>
@@ -891,6 +891,9 @@
   </si>
   <si>
     <t>18.992289</t>
+  </si>
+  <si>
+    <t>-30.01607, 17.572899</t>
   </si>
 </sst>
 </file>
@@ -1440,7 +1443,7 @@
   <dimension ref="A1:N266"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
-      <selection activeCell="G233" sqref="G233"/>
+      <selection activeCell="F233" sqref="F233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6184,12 +6187,14 @@
         <v>8</v>
       </c>
       <c r="E233" s="19">
-        <v>18.172239000000001</v>
+        <v>17.572899</v>
       </c>
       <c r="F233" s="12">
-        <v>-33.269699000000003</v>
-      </c>
-      <c r="G233" s="38"/>
+        <v>-30.016069999999999</v>
+      </c>
+      <c r="G233" s="38" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A234" s="15" t="s">

</xml_diff>